<commit_message>
fix: REsolvendo os problemas do merge
</commit_message>
<xml_diff>
--- a/documentacao/eap-gantt.xlsx
+++ b/documentacao/eap-gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\tiago\faculdade\gerenciamento-software\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2B75FE-B28F-4D4D-B77A-52F2CB91668E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C39038E-CB03-442D-A316-8FC0ADCDCB21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{804ACD51-85FD-475A-949B-B4576FE310A5}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="228">
   <si>
     <t>Nível 1</t>
   </si>
@@ -753,6 +753,9 @@
   </si>
   <si>
     <t>Criação do WebSocket</t>
+  </si>
+  <si>
+    <t>Criação da Lógica de Totalidade</t>
   </si>
 </sst>
 </file>
@@ -968,7 +971,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1815,7 +1818,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{7B9E6FCD-91FA-4847-A1CD-1D89FB9840DD}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="159" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1826,7 +1829,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9633857" cy="5996214"/>
+    <xdr:ext cx="9636824" cy="6006541"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
@@ -2152,13 +2155,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC84F76D-DD96-4E1C-B208-4A56AE55DAAE}">
-  <dimension ref="A1:AK80"/>
+  <dimension ref="A1:AK81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="G72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomRight" activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7789,7 +7792,7 @@
       </c>
       <c r="AJ47" s="1">
         <f>SUMIFS('Horas Trabalhadas'!$D:$D,'Horas Trabalhadas'!$B:$B,$A47,'Horas Trabalhadas'!$C:$C,"&lt;"&amp;Planejamento!AK$1,'Horas Trabalhadas'!$C:$C,"&gt;="&amp;AJ$1)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AK47" s="1">
         <f>SUMIFS('Horas Trabalhadas'!$D:$D,'Horas Trabalhadas'!$B:$B,$A47,'Horas Trabalhadas'!$C:$C,"&lt;"&amp;Planejamento!AL$1,'Horas Trabalhadas'!$C:$C,"&gt;="&amp;AK$1)</f>
@@ -11532,7 +11535,7 @@
       </c>
       <c r="AJ79" s="1">
         <f t="shared" ref="AJ79" si="22">SUM(AJ2:AJ78)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AK79" s="1">
         <f t="shared" ref="AK79" si="23">SUM(AK2:AK78)</f>
@@ -11585,6 +11588,14 @@
       <c r="AA80" s="8">
         <f t="shared" si="24"/>
         <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -11599,8 +11610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB876110-36E2-4389-9494-E58BFAE7ACDB}">
   <dimension ref="A1:G401"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12216,45 +12227,105 @@
       <c r="A28" s="3">
         <v>27</v>
       </c>
+      <c r="B28" s="3">
+        <v>46</v>
+      </c>
+      <c r="C28" s="6">
+        <v>45084</v>
+      </c>
+      <c r="D28" s="3">
+        <v>4</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="G28" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Desenvolvimento/Frontend/UI/Criação da UI de Exércitos Disponíveis</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
+      <c r="B29" s="3">
+        <v>46</v>
+      </c>
+      <c r="C29" s="6">
+        <v>45083</v>
+      </c>
+      <c r="D29" s="3">
+        <v>4</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="G29" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Desenvolvimento/Frontend/UI/Criação da UI de Exércitos Disponíveis</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
+      <c r="B30" s="3">
+        <v>46</v>
+      </c>
+      <c r="C30" s="6">
+        <v>45082</v>
+      </c>
+      <c r="D30" s="3">
+        <v>4</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>199</v>
+      </c>
       <c r="G30" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Desenvolvimento/Frontend/UI/Criação da UI de Exércitos Disponíveis</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
+      <c r="B31" s="3">
+        <v>46</v>
+      </c>
+      <c r="C31" s="6">
+        <v>45083</v>
+      </c>
+      <c r="D31" s="3">
+        <v>4</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="G31" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Desenvolvimento/Frontend/UI/Criação da UI de Exércitos Disponíveis</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>31</v>
       </c>
+      <c r="B32" s="3">
+        <v>46</v>
+      </c>
+      <c r="C32" s="6">
+        <v>45082</v>
+      </c>
+      <c r="D32" s="3">
+        <v>4</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="G32" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Desenvolvimento/Frontend/UI/Criação da UI de Exércitos Disponíveis</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -15769,7 +15840,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="L4" s="3">
         <v>0</v>
@@ -15914,7 +15985,7 @@
       </c>
       <c r="K7" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="L7" s="3">
         <f t="shared" si="3"/>

</xml_diff>